<commit_message>
Adding cost columns to target model
</commit_message>
<xml_diff>
--- a/1_Model/TRG - Projected Occupancy and Costs.xlsx
+++ b/1_Model/TRG - Projected Occupancy and Costs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>ONS.LA.Code</t>
   </si>
@@ -73,6 +73,51 @@
   </si>
   <si>
     <t>Estimated.Self.Funded.Occupancy</t>
+  </si>
+  <si>
+    <t>Res / Nursing</t>
+  </si>
+  <si>
+    <t>Res / Nursing?</t>
+  </si>
+  <si>
+    <t>LA.Avg.Gross.Weekly.Cost.Per.Person</t>
+  </si>
+  <si>
+    <t>Other Supplementary LA Cost Metrics</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>LA.Cost.Of.Care.18-64</t>
+  </si>
+  <si>
+    <t>LA.Cost.Of.Care.65-74</t>
+  </si>
+  <si>
+    <t>LA.Cost.Of.Care.75-84</t>
+  </si>
+  <si>
+    <t>LA.Cost.Of.Care.75pl</t>
+  </si>
+  <si>
+    <t>Estiamted LA-funded occupancy, x LA Avg Gross Weekly Cost of Care</t>
+  </si>
+  <si>
+    <t>TBD!</t>
+  </si>
+  <si>
+    <t>A row for every year between now and 2037</t>
+  </si>
+  <si>
+    <t>~150 LAs</t>
+  </si>
+  <si>
+    <t>From ONS SRC dataset</t>
   </si>
 </sst>
 </file>
@@ -353,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -374,9 +419,11 @@
     <col min="17" max="17" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="21.28515625" customWidth="1"/>
+    <col min="25" max="25" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,6 +480,118 @@
       </c>
       <c r="S1" t="s">
         <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3" t="s">
+        <v>19</v>
+      </c>
+      <c r="W3" t="s">
+        <v>19</v>
+      </c>
+      <c r="X3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U5" t="s">
+        <v>29</v>
+      </c>
+      <c r="V5" t="s">
+        <v>29</v>
+      </c>
+      <c r="W5" t="s">
+        <v>29</v>
+      </c>
+      <c r="X5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>